<commit_message>
Adds Google Scholar of Taiane
</commit_message>
<xml_diff>
--- a/resources/pgc.xlsx
+++ b/resources/pgc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/perfil/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E1E155-B550-5849-8DF1-7CBDFD665E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376113AA-4FA2-9343-B0EE-C7E2A65BEEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>Nome</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>5201325035989406</t>
+  </si>
+  <si>
+    <t>TgSyWIYAAAAJ</t>
   </si>
 </sst>
 </file>
@@ -984,7 +987,7 @@
   <dimension ref="A1:BA50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1635,7 +1638,9 @@
       <c r="B45" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">

</xml_diff>

<commit_message>
Atualização dos docentes credenciados.
</commit_message>
<xml_diff>
--- a/resources/pgc.xlsx
+++ b/resources/pgc.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/perfil/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376113AA-4FA2-9343-B0EE-C7E2A65BEEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B0B9F6-89CE-5B45-AC2D-6576D64E3C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
   <si>
     <t>Nome</t>
   </si>
@@ -620,13 +633,31 @@
   </si>
   <si>
     <t>TgSyWIYAAAAJ</t>
+  </si>
+  <si>
+    <t>João Felipe Nicolaci Pimentel</t>
+  </si>
+  <si>
+    <t>Pedro Cortez Fetter Lopes</t>
+  </si>
+  <si>
+    <t>4603791761884563</t>
+  </si>
+  <si>
+    <t>1rMhTTcAAAAJ</t>
+  </si>
+  <si>
+    <t>7336253957211512</t>
+  </si>
+  <si>
+    <t>qDSsZdgAAAAJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,6 +670,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF555555"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -676,12 +714,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA50"/>
+  <dimension ref="A1:BA52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1400,300 +1439,322 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" t="s">
-        <v>120</v>
-      </c>
-      <c r="C24" t="s">
-        <v>121</v>
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C32" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B33" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C33" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B34" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>191</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>192</v>
+        <v>152</v>
+      </c>
+      <c r="B36" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>155</v>
-      </c>
-      <c r="B37" t="s">
-        <v>156</v>
-      </c>
-      <c r="C37" t="s">
-        <v>157</v>
+        <v>191</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C38" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>196</v>
+        <v>158</v>
+      </c>
+      <c r="B39" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>161</v>
-      </c>
-      <c r="B40" t="s">
-        <v>162</v>
-      </c>
-      <c r="C40" t="s">
-        <v>163</v>
+        <v>194</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B41" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B42" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C42" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>170</v>
-      </c>
-      <c r="B43" t="s">
-        <v>171</v>
-      </c>
-      <c r="C43" t="s">
-        <v>172</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B44" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C44" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>197</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>199</v>
+        <v>170</v>
+      </c>
+      <c r="B45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C46" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47" t="s">
-        <v>180</v>
-      </c>
-      <c r="C47" t="s">
-        <v>181</v>
+        <v>197</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B48" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C48" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B49" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C49" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>185</v>
+      </c>
+      <c r="B51" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>188</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>189</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>190</v>
       </c>
     </row>

</xml_diff>